<commit_message>
Adding CODESSHEET column to Excel
</commit_message>
<xml_diff>
--- a/test_files/Multiple_codelists_and_codes.xlsx
+++ b/test_files/Multiple_codelists_and_codes.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="104">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -28,10 +28,19 @@
     <t>STATUS</t>
   </si>
   <si>
+    <t>BROADER</t>
+  </si>
+  <si>
+    <t>CODESSHEET</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
     <t>PREFLABEL_FI</t>
   </si>
   <si>
-    <t>BROADER</t>
+    <t>HIERARCHYLEVEL</t>
   </si>
   <si>
     <t>PREFLABEL_SV</t>
@@ -40,28 +49,34 @@
     <t>PREFLABEL_EN</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>DEFINITION_FI</t>
   </si>
   <si>
+    <t>DESCRIPTION_FI</t>
+  </si>
+  <si>
+    <t>DESCRIPTION_SV</t>
+  </si>
+  <si>
     <t>DEFINITION_SV</t>
   </si>
   <si>
-    <t>HIERARCHYLEVEL</t>
+    <t>DESCRIPTION_EN</t>
+  </si>
+  <si>
+    <t>SHORTNAME</t>
   </si>
   <si>
     <t>DEFINITION_EN</t>
   </si>
   <si>
-    <t>DESCRIPTION_FI</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_SV</t>
-  </si>
-  <si>
-    <t>DESCRIPTION_EN</t>
+    <t>STARTDATE</t>
+  </si>
+  <si>
+    <t>ENDDATE</t>
+  </si>
+  <si>
+    <t>testikoodi01</t>
   </si>
   <si>
     <t>CHANGENOTE_FI</t>
@@ -73,18 +88,12 @@
     <t>CHANGENOTE_EN</t>
   </si>
   <si>
-    <t>STARTDATE</t>
-  </si>
-  <si>
-    <t>SHORTNAME</t>
-  </si>
-  <si>
-    <t>ENDDATE</t>
-  </si>
-  <si>
     <t>SOURCE</t>
   </si>
   <si>
+    <t>testikoodi11</t>
+  </si>
+  <si>
     <t>LEGALBASE</t>
   </si>
   <si>
@@ -94,9 +103,6 @@
     <t>LICENSE</t>
   </si>
   <si>
-    <t>testikoodi11</t>
-  </si>
-  <si>
     <t>Koodisto7001</t>
   </si>
   <si>
@@ -106,154 +112,160 @@
     <t>DRAFT</t>
   </si>
   <si>
+    <t>Testikoodi 01</t>
+  </si>
+  <si>
+    <t>Kuvaus</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Codes_Koodisto7001</t>
+  </si>
+  <si>
+    <t>koodisto7001</t>
+  </si>
+  <si>
+    <t>Määritelmä</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>yyyyy</t>
+  </si>
+  <si>
+    <t>testikoodi02</t>
+  </si>
+  <si>
+    <t>Testikoodi 02</t>
+  </si>
+  <si>
     <t>Testikoodi 11</t>
   </si>
   <si>
-    <t>Kuvaus</t>
-  </si>
-  <si>
-    <t>Description</t>
+    <t>testikoodi03</t>
+  </si>
+  <si>
+    <t>Testikoodi 03</t>
   </si>
   <si>
     <t>testikoodi12</t>
   </si>
   <si>
+    <t>testikoodi04</t>
+  </si>
+  <si>
     <t>Testikoodi 12</t>
   </si>
   <si>
+    <t>Testikoodi 04</t>
+  </si>
+  <si>
     <t>testikoodi13</t>
   </si>
   <si>
+    <t>testikoodi05</t>
+  </si>
+  <si>
     <t>Testikoodi 13</t>
   </si>
   <si>
+    <t>Testikoodi 05</t>
+  </si>
+  <si>
+    <t>testikoodi06</t>
+  </si>
+  <si>
     <t>testikoodi14</t>
   </si>
   <si>
+    <t>Testikoodi 06</t>
+  </si>
+  <si>
     <t>Testikoodi 14</t>
   </si>
   <si>
+    <t>testikoodi07</t>
+  </si>
+  <si>
+    <t>Koodisto7002</t>
+  </si>
+  <si>
+    <t>Testikoodi 07</t>
+  </si>
+  <si>
+    <t>Codes_Koodisto7002</t>
+  </si>
+  <si>
     <t>testikoodi15</t>
   </si>
   <si>
-    <t>testikoodi01</t>
+    <t>testikoodi08</t>
+  </si>
+  <si>
+    <t>koodisto7002</t>
+  </si>
+  <si>
+    <t>Testikoodi 08</t>
   </si>
   <si>
     <t>Testikoodi 15</t>
   </si>
   <si>
-    <t>Testikoodi 01</t>
+    <t>testikoodi09</t>
   </si>
   <si>
     <t>testikoodi16</t>
   </si>
   <si>
-    <t>testikoodi02</t>
+    <t>Testikoodi 09</t>
   </si>
   <si>
     <t>Testikoodi 16</t>
   </si>
   <si>
-    <t>Testikoodi 02</t>
-  </si>
-  <si>
-    <t>koodisto7001</t>
+    <t>testikoodi10</t>
+  </si>
+  <si>
+    <t>Koodisto7003</t>
+  </si>
+  <si>
+    <t>Testikoodi 10</t>
   </si>
   <si>
     <t>testikoodi17</t>
   </si>
   <si>
-    <t>Määritelmä</t>
-  </si>
-  <si>
-    <t>Definition</t>
+    <t>Codes_Koodisto7003</t>
+  </si>
+  <si>
+    <t>koodisto7003</t>
   </si>
   <si>
     <t>Testikoodi 17</t>
   </si>
   <si>
-    <t>testikoodi03</t>
-  </si>
-  <si>
-    <t>xxxx</t>
-  </si>
-  <si>
-    <t>yyyyy</t>
-  </si>
-  <si>
-    <t>Testikoodi 03</t>
-  </si>
-  <si>
     <t>testikoodi18</t>
   </si>
   <si>
-    <t>testikoodi04</t>
-  </si>
-  <si>
     <t>Testikoodi 18</t>
   </si>
   <si>
-    <t>Testikoodi 04</t>
-  </si>
-  <si>
     <t>testikoodi19</t>
   </si>
   <si>
-    <t>testikoodi05</t>
-  </si>
-  <si>
-    <t>Koodisto7002</t>
-  </si>
-  <si>
     <t>Testikoodi 19</t>
   </si>
   <si>
-    <t>Testikoodi 05</t>
-  </si>
-  <si>
-    <t>koodisto7002</t>
-  </si>
-  <si>
-    <t>testikoodi06</t>
-  </si>
-  <si>
-    <t>Testikoodi 06</t>
-  </si>
-  <si>
     <t>testikoodi20</t>
   </si>
   <si>
-    <t>testikoodi07</t>
-  </si>
-  <si>
     <t>Testikoodi 20</t>
-  </si>
-  <si>
-    <t>Testikoodi 07</t>
-  </si>
-  <si>
-    <t>Koodisto7003</t>
-  </si>
-  <si>
-    <t>testikoodi08</t>
-  </si>
-  <si>
-    <t>koodisto7003</t>
-  </si>
-  <si>
-    <t>Testikoodi 08</t>
-  </si>
-  <si>
-    <t>testikoodi09</t>
-  </si>
-  <si>
-    <t>Testikoodi 09</t>
-  </si>
-  <si>
-    <t>testikoodi10</t>
-  </si>
-  <si>
-    <t>Testikoodi 10</t>
   </si>
   <si>
     <t>testikoodi21</t>
@@ -354,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -364,14 +376,17 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,7 +422,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="11" max="11" width="18.14"/>
+    <col customWidth="1" min="5" max="5" width="23.57"/>
+    <col customWidth="1" min="6" max="6" width="17.14"/>
+    <col customWidth="1" min="7" max="7" width="21.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -424,191 +441,221 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="T1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1">
+        <v>29</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="4">
         <v>1.0</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="2"/>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="G2" s="2"/>
-      <c r="H2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="2"/>
       <c r="N2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" s="5">
+        <v>34</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="6">
         <v>43161.0</v>
       </c>
-      <c r="R2" s="5">
+      <c r="S2" s="6">
         <v>43189.0</v>
       </c>
-      <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="1">
+        <v>59</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="4">
         <v>1.0</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="2"/>
       <c r="K3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="2"/>
       <c r="N3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q3" s="5">
+        <v>34</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R3" s="6">
         <v>43162.0</v>
       </c>
-      <c r="R3" s="5">
+      <c r="S3" s="6">
         <v>43190.0</v>
       </c>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1">
+      <c r="B4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="4">
         <v>1.0</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="2"/>
       <c r="K4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>32</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="2"/>
       <c r="N4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q4" s="5">
+        <v>34</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" s="6">
         <v>43163.0</v>
       </c>
-      <c r="R4" s="5">
+      <c r="S4" s="6">
         <v>43191.0</v>
       </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -630,356 +677,356 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="1" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="M2" s="3">
+      <c r="M2" s="5">
         <v>43133.0</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="5">
         <v>43352.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L3" s="2"/>
-      <c r="M3" s="3">
+      <c r="M3" s="5">
         <v>43134.0</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="5">
         <v>43353.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L4" s="2"/>
-      <c r="M4" s="3">
+      <c r="M4" s="5">
         <v>43135.0</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="5">
         <v>43354.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="3">
+      <c r="M5" s="5">
         <v>43136.0</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="5">
         <v>43355.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="3">
+      <c r="M6" s="5">
         <v>43137.0</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="5">
         <v>43356.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="3">
+      <c r="M7" s="5">
         <v>43138.0</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="5">
         <v>43357.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="3">
+      <c r="M8" s="5">
         <v>43139.0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="5">
         <v>43358.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L9" s="2"/>
-      <c r="M9" s="3">
+      <c r="M9" s="5">
         <v>43140.0</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="5">
         <v>43359.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L10" s="2"/>
-      <c r="M10" s="3">
+      <c r="M10" s="5">
         <v>43141.0</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="5">
         <v>43360.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L11" s="2"/>
-      <c r="M11" s="3">
+      <c r="M11" s="5">
         <v>43142.0</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="5">
         <v>43361.0</v>
       </c>
     </row>
@@ -1003,356 +1050,356 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="M2" s="3">
+      <c r="M2" s="5">
         <v>43133.0</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="5">
         <v>43352.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L3" s="2"/>
-      <c r="M3" s="3">
+      <c r="M3" s="5">
         <v>43134.0</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="5">
         <v>43353.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L4" s="2"/>
-      <c r="M4" s="3">
+      <c r="M4" s="5">
         <v>43135.0</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="5">
         <v>43354.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="3">
+      <c r="M5" s="5">
         <v>43136.0</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="5">
         <v>43355.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="3">
+      <c r="M6" s="5">
         <v>43137.0</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="5">
         <v>43356.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="3">
+      <c r="M7" s="5">
         <v>43138.0</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="5">
         <v>43357.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="3">
+      <c r="M8" s="5">
         <v>43139.0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="5">
         <v>43358.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L9" s="2"/>
-      <c r="M9" s="3">
+      <c r="M9" s="5">
         <v>43140.0</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="5">
         <v>43359.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L10" s="2"/>
-      <c r="M10" s="3">
+      <c r="M10" s="5">
         <v>43141.0</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="5">
         <v>43360.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L11" s="2"/>
-      <c r="M11" s="3">
+      <c r="M11" s="5">
         <v>43142.0</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="5">
         <v>43361.0</v>
       </c>
     </row>
@@ -1376,356 +1423,356 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L2" s="2"/>
-      <c r="M2" s="3">
+      <c r="M2" s="5">
         <v>43133.0</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="5">
         <v>43352.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="1" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
       <c r="I3" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L3" s="2"/>
-      <c r="M3" s="3">
+      <c r="M3" s="5">
         <v>43134.0</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="5">
         <v>43353.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="1" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L4" s="2"/>
-      <c r="M4" s="3">
+      <c r="M4" s="5">
         <v>43135.0</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="5">
         <v>43354.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L5" s="2"/>
-      <c r="M5" s="3">
+      <c r="M5" s="5">
         <v>43136.0</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="5">
         <v>43355.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="1" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L6" s="2"/>
-      <c r="M6" s="3">
+      <c r="M6" s="5">
         <v>43137.0</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="5">
         <v>43356.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="1" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L7" s="2"/>
-      <c r="M7" s="3">
+      <c r="M7" s="5">
         <v>43138.0</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="5">
         <v>43357.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L8" s="2"/>
-      <c r="M8" s="3">
+      <c r="M8" s="5">
         <v>43139.0</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="5">
         <v>43358.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="1" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L9" s="2"/>
-      <c r="M9" s="3">
+      <c r="M9" s="5">
         <v>43140.0</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="5">
         <v>43359.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L10" s="2"/>
-      <c r="M10" s="3">
+      <c r="M10" s="5">
         <v>43141.0</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="5">
         <v>43360.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="1" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="L11" s="2"/>
-      <c r="M11" s="3">
+      <c r="M11" s="5">
         <v>43142.0</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="5">
         <v>43361.0</v>
       </c>
     </row>

</xml_diff>